<commit_message>
Atualiza o levantamento de requisitos
</commit_message>
<xml_diff>
--- a/documentacao/levantamento-requisitos.xlsx
+++ b/documentacao/levantamento-requisitos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Listar produtos</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Cadastrar dados do aluno</t>
   </si>
   <si>
-    <t>Administrador visualiza informações dos pedidos</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -57,6 +54,69 @@
   </si>
   <si>
     <t>RF003</t>
+  </si>
+  <si>
+    <t>Cadastrar produto</t>
+  </si>
+  <si>
+    <t>Editar produto</t>
+  </si>
+  <si>
+    <t>Visualizar detalhes do produto</t>
+  </si>
+  <si>
+    <t>RF004</t>
+  </si>
+  <si>
+    <t>Exibir informações de contato</t>
+  </si>
+  <si>
+    <t>Exibir mensagem de confirmação do pedido</t>
+  </si>
+  <si>
+    <t>Definir disponível ou indisponível</t>
+  </si>
+  <si>
+    <t>Definir poucas unidades</t>
+  </si>
+  <si>
+    <t>Visualizar pedidos</t>
+  </si>
+  <si>
+    <t>Efetuar login</t>
+  </si>
+  <si>
+    <t>Somente administrador pode acessar o sistema web</t>
+  </si>
+  <si>
+    <t>Disponibilizar o aplicativo nas plataformas Windows Phone, Android e iOs</t>
+  </si>
+  <si>
+    <t>RF005</t>
+  </si>
+  <si>
+    <t>RF006</t>
+  </si>
+  <si>
+    <t>RF007</t>
+  </si>
+  <si>
+    <t>RF008</t>
+  </si>
+  <si>
+    <t>RN001</t>
+  </si>
+  <si>
+    <t>RNF001</t>
+  </si>
+  <si>
+    <t>RNF002</t>
+  </si>
+  <si>
+    <t>RNF003</t>
+  </si>
+  <si>
+    <t>RF009</t>
   </si>
 </sst>
 </file>
@@ -405,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,102 +498,180 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="4"/>
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>